<commit_message>
objects and collections export OK. abandon jdbc resultsets.
</commit_message>
<xml_diff>
--- a/examples/template.xlsx
+++ b/examples/template.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name:</t>
   </si>
@@ -62,6 +63,18 @@
   </si>
   <si>
     <t>${obj.cols.v}</t>
+  </si>
+  <si>
+    <t>${myCollection.color}</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>${myCollection.value}</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -487,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -510,4 +523,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>